<commit_message>
2.1.2: Adapt to new generics support on blancoCg.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectTask.xlsx
+++ b/meta/program/BlancoValueObjectTask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObject/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C79E4F-3E18-5E45-9C94-A5644306877A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2488E591-A6DE-6C4E-870E-503B79D11084}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -460,6 +460,23 @@
       <t xml:space="preserve">イガイノ </t>
     </rPh>
     <rPh sb="17" eb="19">
+      <t xml:space="preserve">ムシシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>ignoreImport</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Java向け以外のインポートを無視します。</t>
+    <rPh sb="4" eb="5">
+      <t xml:space="preserve">ムケ </t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t xml:space="preserve">イガイノ </t>
+    </rPh>
+    <rPh sb="15" eb="17">
       <t xml:space="preserve">ムシシマス。 </t>
     </rPh>
     <phoneticPr fontId="5"/>
@@ -1496,10 +1513,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1801,7 +1818,7 @@
     </row>
     <row r="21" spans="1:10" ht="52" customHeight="1">
       <c r="A21" s="49">
-        <f t="shared" ref="A21:A28" si="0">A20+1</f>
+        <f t="shared" ref="A21:A29" si="0">A20+1</f>
         <v>8</v>
       </c>
       <c r="B21" s="23" t="s">
@@ -1970,16 +1987,28 @@
       <c r="I28" s="68"/>
       <c r="J28" s="69"/>
     </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="22"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="27"/>
+    <row r="29" spans="1:10" s="70" customFormat="1">
+      <c r="A29" s="64">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B29" s="75" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="66"/>
+      <c r="E29" s="67" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
+      <c r="J29" s="69"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="22"/>
@@ -2004,15 +2033,26 @@
       <c r="I31" s="27"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="28"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="33"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="27"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -2034,17 +2074,17 @@
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F48" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F49" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D20 D29:D32 D22:D23" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D20 D30:D33 D22:D23" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>必須</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C32" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C33" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>型リスト</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D24:D28" xr:uid="{DB2CD47E-33DA-5C40-81E3-C2A567C8D0F1}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D24:D29" xr:uid="{DB2CD47E-33DA-5C40-81E3-C2A567C8D0F1}">
       <formula1>必須</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>